<commit_message>
File support in excel source.
</commit_message>
<xml_diff>
--- a/sources/excel/sample-data.xlsx
+++ b/sources/excel/sample-data.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\fruit_to_lime\bin\hubbabubba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\go-org-import-debug\file-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Företag" sheetId="1" r:id="rId1"/>
-    <sheet name="Kontaktperson" sheetId="2" r:id="rId2"/>
-    <sheet name="Anteckningar" sheetId="3" r:id="rId3"/>
-    <sheet name="Medarbetare" sheetId="4" r:id="rId4"/>
+    <sheet name="Dokument" sheetId="5" r:id="rId2"/>
+    <sheet name="Kontaktperson" sheetId="2" r:id="rId3"/>
+    <sheet name="Anteckningar" sheetId="3" r:id="rId4"/>
+    <sheet name="Medarbetare" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Företag!$A$1:$E$955</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Kontaktperson!$A$1:$E$902</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Kontaktperson!$A$1:$E$902</definedName>
     <definedName name="company" localSheetId="0">Företag!$A$2:$E$955</definedName>
-    <definedName name="contact_person" localSheetId="1">Kontaktperson!$A$2:$E$902</definedName>
-    <definedName name="note" localSheetId="2">Anteckningar!$A$2:$AF$2390</definedName>
+    <definedName name="contact_person" localSheetId="2">Kontaktperson!$A$2:$E$902</definedName>
+    <definedName name="note" localSheetId="3">Anteckningar!$A$2:$AF$2390</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Namn</t>
   </si>
@@ -155,6 +156,51 @@
   </si>
   <si>
     <t>vincent.vega@lundalogik.se</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Företag</t>
+  </si>
+  <si>
+    <t>Offert</t>
+  </si>
+  <si>
+    <t>Nu fläskar vi på ordentligt</t>
+  </si>
+  <si>
+    <t>offert.docx</t>
+  </si>
+  <si>
+    <t>Avtal</t>
+  </si>
+  <si>
+    <t>Skickar detta för underskrift</t>
+  </si>
+  <si>
+    <t>avtal.docx</t>
+  </si>
+  <si>
+    <t>Får fundera på detta</t>
+  </si>
+  <si>
+    <t>offert-2.docx</t>
+  </si>
+  <si>
+    <t>Kör bara kör</t>
+  </si>
+  <si>
+    <t>more/offert-2.pdf</t>
+  </si>
+  <si>
+    <t>more\avtal.docx</t>
+  </si>
+  <si>
+    <t>Skapad Av</t>
   </si>
 </sst>
 </file>
@@ -515,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -570,6 +616,129 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E892"/>
   <sheetViews>
@@ -893,12 +1062,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8133,7 +8302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update excel source sample file
</commit_message>
<xml_diff>
--- a/sources/excel/sample-data.xlsx
+++ b/sources/excel/sample-data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\move-to-go\mytests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9BE076C8-437C-4410-A68D-946178F89EB5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11988" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11988" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Företag" sheetId="1" r:id="rId1"/>
@@ -40,8 +41,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="company" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="company" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\company.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="5">
         <textField/>
@@ -52,7 +53,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="contact_person" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="contact_person" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\contact_person.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="5">
         <textField/>
@@ -63,7 +64,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="note" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="note" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\note.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="4">
         <textField/>
@@ -73,7 +74,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="note1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="note1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\note.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="4">
         <textField/>
@@ -83,7 +84,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="note11" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="note11" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\note.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="4">
         <textField/>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Namn</t>
   </si>
@@ -284,14 +285,23 @@
   <si>
     <t>Rubrik</t>
   </si>
+  <si>
+    <t>MailConsent</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nej</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ hh:mm;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ hh:mm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -357,10 +367,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,23 +387,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="company" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="company" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="contact_person" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="contact_person" connectionId="2" xr16:uid="{00000000-0016-0000-0300-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="note" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="note" connectionId="3" xr16:uid="{00000000-0016-0000-0500-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="note" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="note" connectionId="4" xr16:uid="{00000000-0016-0000-0600-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="note" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="note" connectionId="5" xr16:uid="{00000000-0016-0000-0700-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -658,7 +668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -710,13 +720,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E955"/>
+  <autoFilter ref="A1:E955" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -839,7 +849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -913,19 +923,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E892"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F892"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,7 +947,7 @@
     <col min="5" max="5" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -953,8 +963,11 @@
       <c r="E1" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -970,8 +983,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -988,7 +1004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1004,6 +1020,9 @@
       <c r="E4">
         <v>3</v>
       </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D77" s="1"/>
@@ -1234,18 +1253,18 @@
       <c r="D892" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E902"/>
+  <autoFilter ref="A1:E902" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1320,8 +1339,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1329,7 +1348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8569,7 +8588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H2390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15846,10 +15865,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I2390"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added the possibility to convert Mail consents to be imported to Lime Go
* Handle email consent in Lime Easy
* Add example for email consent into excel
* Update excel source sample file
* The consent file is not constant, and should be editable in the converter.
</commit_message>
<xml_diff>
--- a/sources/excel/sample-data.xlsx
+++ b/sources/excel/sample-data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\move-to-go\mytests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9BE076C8-437C-4410-A68D-946178F89EB5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11988" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11988" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Företag" sheetId="1" r:id="rId1"/>
@@ -40,8 +41,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="company" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="company" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\company.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="5">
         <textField/>
@@ -52,7 +53,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="contact_person" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="contact_person" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\contact_person.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="5">
         <textField/>
@@ -63,7 +64,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="note" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="note" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\note.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="4">
         <textField/>
@@ -73,7 +74,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="note1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="note1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\note.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="4">
         <textField/>
@@ -83,7 +84,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="note11" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="note11" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Downloads\note.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="4">
         <textField/>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Namn</t>
   </si>
@@ -284,14 +285,23 @@
   <si>
     <t>Rubrik</t>
   </si>
+  <si>
+    <t>MailConsent</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nej</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ hh:mm;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ hh:mm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -357,10 +367,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,23 +387,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="company" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="company" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="contact_person" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="contact_person" connectionId="2" xr16:uid="{00000000-0016-0000-0300-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="note" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="note" connectionId="3" xr16:uid="{00000000-0016-0000-0500-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="note" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="note" connectionId="4" xr16:uid="{00000000-0016-0000-0600-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="note" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="note" connectionId="5" xr16:uid="{00000000-0016-0000-0700-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -658,7 +668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -710,13 +720,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E955"/>
+  <autoFilter ref="A1:E955" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -839,7 +849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -913,19 +923,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E892"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F892"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,7 +947,7 @@
     <col min="5" max="5" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -953,8 +963,11 @@
       <c r="E1" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -970,8 +983,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -988,7 +1004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1004,6 +1020,9 @@
       <c r="E4">
         <v>3</v>
       </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D77" s="1"/>
@@ -1234,18 +1253,18 @@
       <c r="D892" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E902"/>
+  <autoFilter ref="A1:E902" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1320,8 +1339,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1329,7 +1348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8569,7 +8588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H2390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15846,10 +15865,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I2390"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>